<commit_message>
change dimmension of battery and case
</commit_message>
<xml_diff>
--- a/dimmensions.xlsx
+++ b/dimmensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Projects\WearableWLED\WearableWLED_Mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647ECA83-D457-492F-B27A-72189EFCBBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392D21A9-F4CD-4693-87FC-F9D66EBAA4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>

</xml_diff>